<commit_message>
Implement views for recording tests and test results
</commit_message>
<xml_diff>
--- a/sure/tests/data/SURE_Q.xlsx
+++ b/sure/tests/data/SURE_Q.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CLIENT" sheetId="1" state="visible" r:id="rId3"/>
@@ -1542,15 +1542,7 @@
 (If the client has provided their mobile phone number, they will receive a reminder.)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1: 2 weeks
+    <t xml:space="preserve">1: 2 weeks
 2: 4 weeks
 3: 6 weeks
 4: 2 months
@@ -1559,19 +1551,7 @@
 7: 9 months
 8: 12 months
 97: No reminder useful
-99: </t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">missing</t>
-    </r>
+99: missing</t>
   </si>
   <si>
     <t xml:space="preserve">TESTS-PERFORMED</t>
@@ -1707,10 +1687,10 @@
     <t xml:space="preserve">Information by SMS</t>
   </si>
   <si>
-    <t xml:space="preserve">Information Text (negativ)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Information Text (positiv)</t>
+    <t xml:space="preserve">Information Text (negative)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Information Text (reactive)</t>
   </si>
   <si>
     <t xml:space="preserve">Information Text (unclear)</t>
@@ -3184,356 +3164,360 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="171">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="14" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="5" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="15" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="15" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3541,11 +3525,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="7" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3553,315 +3537,315 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="15" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="15" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="16" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="16" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="15" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="15" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="15" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="15" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="15" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="15" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="15" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="15" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="9" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="9" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="15" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="15" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="15" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="15" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="15" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="15" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="35" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="32" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="36" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="36" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="37" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="37" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="5" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="5" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="43" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="44" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4117,7 +4101,7 @@
   </sheetPr>
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -5404,25 +5388,25 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="78.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="73" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="73" width="31.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="73" width="28.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="73" width="78.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="73" width="27.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="73" width="36.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="76" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
@@ -5430,140 +5414,140 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="77" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="78" t="s">
         <v>182</v>
       </c>
-      <c r="C2" s="77" t="s">
+      <c r="C2" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="79" t="s">
         <v>183</v>
       </c>
-      <c r="E2" s="78"/>
+      <c r="E2" s="79"/>
     </row>
     <row r="3" customFormat="false" ht="151.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="80" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="81" t="s">
         <v>186</v>
       </c>
-      <c r="D3" s="81" t="s">
+      <c r="D3" s="82" t="s">
         <v>187</v>
       </c>
-      <c r="E3" s="81"/>
-      <c r="F3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="83"/>
     </row>
     <row r="4" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="80" t="s">
         <v>188</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="81" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="81" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="82" t="s">
         <v>190</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="84" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="151.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="80" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="80" t="s">
+      <c r="B5" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="81" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="84" t="s">
+      <c r="D5" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="E5" s="84"/>
-    </row>
-    <row r="6" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="85" t="s">
+      <c r="E5" s="85"/>
+    </row>
+    <row r="6" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="E6" s="84"/>
+      <c r="E6" s="85"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="86" t="s">
+      <c r="A7" s="87" t="s">
         <v>197</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="88" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="D7" s="88" t="s">
+      <c r="D7" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="E7" s="88"/>
+      <c r="E7" s="89"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="90" t="s">
         <v>200</v>
       </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="91" t="s">
+      <c r="B8" s="91"/>
+      <c r="C8" s="92" t="s">
         <v>199</v>
       </c>
-      <c r="D8" s="91" t="s">
+      <c r="D8" s="92" t="s">
         <v>199</v>
       </c>
-      <c r="E8" s="91"/>
+      <c r="E8" s="92"/>
     </row>
     <row r="9" customFormat="false" ht="48.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="92" t="s">
+      <c r="A9" s="93" t="s">
         <v>201</v>
       </c>
-      <c r="B9" s="93" t="s">
+      <c r="B9" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="95" t="s">
         <v>203</v>
       </c>
-      <c r="E9" s="94"/>
+      <c r="E9" s="95"/>
     </row>
     <row r="10" customFormat="false" ht="26.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="79" t="s">
+      <c r="A10" s="80" t="s">
         <v>204</v>
       </c>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="81" t="s">
         <v>206</v>
       </c>
-      <c r="D10" s="81" t="s">
+      <c r="D10" s="82" t="s">
         <v>207</v>
       </c>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="96" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5591,1715 +5575,1715 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="96" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="96" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="97" width="48.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="96" width="30.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="96" width="44.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="96" width="24.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="12" style="96" width="57.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="97" width="51.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="17" style="96" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="97" width="11.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="97" width="7.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="98" width="48.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="97" width="30.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="97" width="44.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="97" width="24.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="12" style="97" width="57.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="98" width="51.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="17" style="97" width="11.44"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="98"/>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="99"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-    </row>
-    <row r="2" s="96" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="103" t="s">
+      <c r="A1" s="99"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+    </row>
+    <row r="2" s="97" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="104" t="s">
         <v>208</v>
       </c>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="105" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="105" t="s">
+      <c r="C2" s="106" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="106" t="s">
+      <c r="D2" s="107" t="s">
         <v>211</v>
       </c>
-      <c r="E2" s="106" t="s">
+      <c r="E2" s="107" t="s">
         <v>212</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="108" t="s">
         <v>213</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="109" t="s">
         <v>214</v>
       </c>
-      <c r="H2" s="109" t="s">
+      <c r="H2" s="110" t="s">
         <v>215</v>
       </c>
-      <c r="I2" s="110" t="s">
+      <c r="I2" s="111" t="s">
         <v>216</v>
       </c>
-      <c r="J2" s="110" t="s">
+      <c r="J2" s="111" t="s">
         <v>217</v>
       </c>
-      <c r="K2" s="111" t="s">
+      <c r="K2" s="112" t="s">
         <v>218</v>
       </c>
-      <c r="L2" s="112" t="s">
+      <c r="L2" s="113" t="s">
         <v>219</v>
       </c>
-      <c r="M2" s="112" t="s">
+      <c r="M2" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="N2" s="112" t="s">
+      <c r="N2" s="113" t="s">
         <v>221</v>
       </c>
-      <c r="O2" s="112" t="s">
+      <c r="O2" s="113" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="113"/>
-      <c r="B3" s="114"/>
-      <c r="C3" s="115"/>
-      <c r="D3" s="115"/>
-      <c r="E3" s="115"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="117" t="n">
+      <c r="A3" s="114"/>
+      <c r="B3" s="115"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="117"/>
+      <c r="G3" s="118" t="n">
         <v>1</v>
       </c>
-      <c r="H3" s="118" t="s">
+      <c r="H3" s="119" t="s">
         <v>223</v>
       </c>
-      <c r="I3" s="119"/>
-      <c r="J3" s="120"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
+      <c r="M3" s="123"/>
+      <c r="N3" s="123"/>
+      <c r="O3" s="123"/>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="123" t="s">
+      <c r="A4" s="124" t="s">
         <v>224</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="125" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="125" t="s">
+      <c r="C4" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="D4" s="125" t="s">
+      <c r="D4" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="125" t="s">
+      <c r="E4" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="F4" s="125" t="s">
+      <c r="F4" s="126" t="s">
         <v>224</v>
       </c>
-      <c r="G4" s="126" t="n">
+      <c r="G4" s="127" t="n">
         <v>11</v>
       </c>
-      <c r="H4" s="127" t="s">
+      <c r="H4" s="128" t="s">
         <v>225</v>
       </c>
-      <c r="I4" s="128"/>
-      <c r="J4" s="129" t="s">
+      <c r="I4" s="129"/>
+      <c r="J4" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="K4" s="130" t="s">
+      <c r="K4" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L4" s="130" t="s">
+      <c r="L4" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="M4" s="131" t="s">
+      <c r="M4" s="132" t="s">
         <v>229</v>
       </c>
-      <c r="N4" s="132"/>
-      <c r="O4" s="132"/>
-      <c r="P4" s="133" t="s">
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="134" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="134"/>
-      <c r="B5" s="135"/>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
-      <c r="F5" s="136"/>
-      <c r="G5" s="126" t="n">
+      <c r="A5" s="135"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="137"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="127" t="n">
         <v>12</v>
       </c>
-      <c r="H5" s="127" t="s">
+      <c r="H5" s="128" t="s">
         <v>231</v>
       </c>
-      <c r="I5" s="137" t="s">
+      <c r="I5" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J5" s="128"/>
-      <c r="K5" s="132"/>
-      <c r="L5" s="132"/>
-      <c r="M5" s="132"/>
-      <c r="N5" s="132"/>
-      <c r="O5" s="132"/>
+      <c r="J5" s="129"/>
+      <c r="K5" s="133"/>
+      <c r="L5" s="133"/>
+      <c r="M5" s="133"/>
+      <c r="N5" s="133"/>
+      <c r="O5" s="133"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="134"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="136"/>
-      <c r="D6" s="136"/>
-      <c r="E6" s="136"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="126" t="n">
+      <c r="A6" s="135"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="127" t="n">
         <v>13</v>
       </c>
-      <c r="H6" s="127" t="s">
+      <c r="H6" s="128" t="s">
         <v>233</v>
       </c>
-      <c r="I6" s="137" t="s">
+      <c r="I6" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J6" s="128"/>
-      <c r="K6" s="132"/>
-      <c r="L6" s="132"/>
-      <c r="M6" s="132"/>
-      <c r="N6" s="132"/>
-      <c r="O6" s="132"/>
+      <c r="J6" s="129"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="134"/>
-      <c r="B7" s="135"/>
-      <c r="C7" s="136"/>
-      <c r="D7" s="136"/>
-      <c r="E7" s="136"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="126" t="n">
+      <c r="A7" s="135"/>
+      <c r="B7" s="136"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="139"/>
+      <c r="G7" s="127" t="n">
         <v>14</v>
       </c>
-      <c r="H7" s="127" t="s">
+      <c r="H7" s="128" t="s">
         <v>234</v>
       </c>
-      <c r="I7" s="128"/>
-      <c r="J7" s="129" t="s">
+      <c r="I7" s="129"/>
+      <c r="J7" s="130" t="s">
         <v>235</v>
       </c>
-      <c r="K7" s="130" t="s">
+      <c r="K7" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L7" s="130" t="s">
+      <c r="L7" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M7" s="132"/>
-      <c r="N7" s="132"/>
-      <c r="O7" s="132"/>
+      <c r="M7" s="133"/>
+      <c r="N7" s="133"/>
+      <c r="O7" s="133"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="134"/>
-      <c r="B8" s="135"/>
-      <c r="C8" s="136"/>
-      <c r="D8" s="136"/>
-      <c r="E8" s="136"/>
-      <c r="F8" s="138"/>
-      <c r="G8" s="126" t="n">
+      <c r="A8" s="135"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="137"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="137"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="127" t="n">
         <v>15</v>
       </c>
-      <c r="H8" s="127" t="s">
+      <c r="H8" s="128" t="s">
         <v>237</v>
       </c>
-      <c r="I8" s="128"/>
-      <c r="J8" s="137" t="s">
+      <c r="I8" s="129"/>
+      <c r="J8" s="138" t="s">
         <v>238</v>
       </c>
-      <c r="K8" s="130" t="s">
+      <c r="K8" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="130" t="s">
+      <c r="L8" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M8" s="132"/>
-      <c r="N8" s="132"/>
-      <c r="O8" s="132"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="139"/>
-      <c r="B9" s="140"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="142"/>
-      <c r="G9" s="143" t="n">
+      <c r="A9" s="140"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="144" t="n">
         <v>2</v>
       </c>
-      <c r="H9" s="144" t="s">
+      <c r="H9" s="145" t="s">
         <v>239</v>
       </c>
-      <c r="I9" s="145"/>
-      <c r="J9" s="145"/>
-      <c r="K9" s="122"/>
-      <c r="L9" s="122"/>
-      <c r="M9" s="122"/>
-      <c r="N9" s="122"/>
-      <c r="O9" s="122"/>
-    </row>
-    <row r="10" s="96" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="134" t="s">
+      <c r="I9" s="146"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="123"/>
+      <c r="L9" s="123"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="123"/>
+      <c r="O9" s="123"/>
+    </row>
+    <row r="10" s="97" customFormat="true" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="B10" s="135" t="s">
+      <c r="B10" s="136" t="s">
         <v>224</v>
       </c>
-      <c r="C10" s="136"/>
-      <c r="D10" s="136" t="s">
+      <c r="C10" s="137"/>
+      <c r="D10" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E10" s="136"/>
-      <c r="F10" s="138" t="s">
+      <c r="E10" s="137"/>
+      <c r="F10" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G10" s="126" t="n">
+      <c r="G10" s="127" t="n">
         <v>21</v>
       </c>
-      <c r="H10" s="127" t="s">
+      <c r="H10" s="128" t="s">
         <v>240</v>
       </c>
-      <c r="I10" s="128"/>
-      <c r="J10" s="129" t="s">
+      <c r="I10" s="129"/>
+      <c r="J10" s="130" t="s">
         <v>241</v>
       </c>
-      <c r="K10" s="130" t="s">
+      <c r="K10" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="130" t="s">
+      <c r="L10" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M10" s="146" t="s">
+      <c r="M10" s="147" t="s">
         <v>243</v>
       </c>
-      <c r="N10" s="147" t="s">
+      <c r="N10" s="148" t="s">
         <v>244</v>
       </c>
-      <c r="O10" s="132"/>
+      <c r="O10" s="133"/>
     </row>
     <row r="11" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="134"/>
-      <c r="B11" s="135"/>
-      <c r="C11" s="136" t="s">
+      <c r="A11" s="135"/>
+      <c r="B11" s="136"/>
+      <c r="C11" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="138"/>
-      <c r="G11" s="126" t="n">
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="139"/>
+      <c r="G11" s="127" t="n">
         <v>22</v>
       </c>
-      <c r="H11" s="127" t="s">
+      <c r="H11" s="128" t="s">
         <v>245</v>
       </c>
-      <c r="I11" s="128"/>
-      <c r="J11" s="129" t="s">
+      <c r="I11" s="129"/>
+      <c r="J11" s="130" t="s">
         <v>246</v>
       </c>
-      <c r="K11" s="130" t="s">
+      <c r="K11" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="130" t="s">
+      <c r="L11" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M11" s="146"/>
-      <c r="N11" s="147"/>
-      <c r="O11" s="148" t="s">
+      <c r="M11" s="147"/>
+      <c r="N11" s="148"/>
+      <c r="O11" s="149" t="s">
         <v>247</v>
       </c>
-      <c r="P11" s="149"/>
+      <c r="P11" s="150"/>
     </row>
     <row r="12" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="134"/>
-      <c r="B12" s="135"/>
-      <c r="C12" s="136" t="s">
+      <c r="A12" s="135"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="D12" s="136"/>
-      <c r="E12" s="136"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="126" t="n">
+      <c r="D12" s="137"/>
+      <c r="E12" s="137"/>
+      <c r="F12" s="139"/>
+      <c r="G12" s="127" t="n">
         <v>23</v>
       </c>
-      <c r="H12" s="127" t="s">
+      <c r="H12" s="128" t="s">
         <v>248</v>
       </c>
-      <c r="I12" s="128"/>
-      <c r="J12" s="129" t="s">
+      <c r="I12" s="129"/>
+      <c r="J12" s="130" t="s">
         <v>249</v>
       </c>
-      <c r="K12" s="130" t="s">
+      <c r="K12" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="130" t="s">
+      <c r="L12" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M12" s="146"/>
-      <c r="N12" s="147"/>
-      <c r="O12" s="148"/>
-      <c r="P12" s="149"/>
+      <c r="M12" s="147"/>
+      <c r="N12" s="148"/>
+      <c r="O12" s="149"/>
+      <c r="P12" s="150"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="134"/>
-      <c r="B13" s="135"/>
-      <c r="C13" s="136"/>
-      <c r="D13" s="136"/>
-      <c r="E13" s="136"/>
-      <c r="F13" s="138"/>
-      <c r="G13" s="126" t="n">
+      <c r="A13" s="135"/>
+      <c r="B13" s="136"/>
+      <c r="C13" s="137"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="137"/>
+      <c r="F13" s="139"/>
+      <c r="G13" s="127" t="n">
         <v>24</v>
       </c>
-      <c r="H13" s="127" t="s">
+      <c r="H13" s="128" t="s">
         <v>250</v>
       </c>
-      <c r="I13" s="137" t="s">
+      <c r="I13" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J13" s="128"/>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
-      <c r="M13" s="132"/>
-      <c r="N13" s="132"/>
-      <c r="O13" s="132"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="133"/>
+      <c r="M13" s="133"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="133"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="134"/>
-      <c r="B14" s="135"/>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="E14" s="136"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="126" t="n">
+      <c r="A14" s="135"/>
+      <c r="B14" s="136"/>
+      <c r="C14" s="137"/>
+      <c r="D14" s="137"/>
+      <c r="E14" s="137"/>
+      <c r="F14" s="139"/>
+      <c r="G14" s="127" t="n">
         <v>25</v>
       </c>
-      <c r="H14" s="127" t="s">
+      <c r="H14" s="128" t="s">
         <v>251</v>
       </c>
-      <c r="I14" s="128"/>
-      <c r="J14" s="137" t="s">
+      <c r="I14" s="129"/>
+      <c r="J14" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K14" s="130" t="s">
+      <c r="K14" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L14" s="130" t="s">
+      <c r="L14" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M14" s="132"/>
-      <c r="N14" s="132"/>
-      <c r="O14" s="132"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="133"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="139"/>
-      <c r="B15" s="140"/>
-      <c r="C15" s="141"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="143" t="n">
+      <c r="A15" s="140"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="142"/>
+      <c r="D15" s="142"/>
+      <c r="E15" s="142"/>
+      <c r="F15" s="143"/>
+      <c r="G15" s="144" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="144" t="s">
+      <c r="H15" s="145" t="s">
         <v>252</v>
       </c>
-      <c r="I15" s="145"/>
-      <c r="J15" s="150"/>
-      <c r="K15" s="122"/>
-      <c r="L15" s="122"/>
-      <c r="M15" s="122"/>
-      <c r="N15" s="122"/>
-      <c r="O15" s="122"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="151"/>
+      <c r="K15" s="123"/>
+      <c r="L15" s="123"/>
+      <c r="M15" s="123"/>
+      <c r="N15" s="123"/>
+      <c r="O15" s="123"/>
     </row>
     <row r="16" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="135" t="s">
+      <c r="B16" s="136" t="s">
         <v>224</v>
       </c>
-      <c r="C16" s="136" t="s">
+      <c r="C16" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="D16" s="136" t="s">
+      <c r="D16" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E16" s="136"/>
-      <c r="F16" s="138" t="s">
+      <c r="E16" s="137"/>
+      <c r="F16" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G16" s="126" t="n">
+      <c r="G16" s="127" t="n">
         <v>31</v>
       </c>
-      <c r="H16" s="127" t="s">
+      <c r="H16" s="128" t="s">
         <v>253</v>
       </c>
-      <c r="I16" s="128"/>
-      <c r="J16" s="137" t="s">
+      <c r="I16" s="129"/>
+      <c r="J16" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K16" s="130" t="s">
+      <c r="K16" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L16" s="130" t="s">
+      <c r="L16" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M16" s="151" t="s">
+      <c r="M16" s="152" t="s">
         <v>254</v>
       </c>
-      <c r="N16" s="147" t="s">
+      <c r="N16" s="148" t="s">
         <v>255</v>
       </c>
-      <c r="O16" s="132"/>
+      <c r="O16" s="133"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="134"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="136"/>
-      <c r="E17" s="136"/>
-      <c r="F17" s="138"/>
-      <c r="G17" s="126" t="n">
+      <c r="A17" s="135"/>
+      <c r="B17" s="136"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
+      <c r="E17" s="137"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="127" t="n">
         <v>32</v>
       </c>
-      <c r="H17" s="127" t="s">
+      <c r="H17" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="I17" s="128"/>
-      <c r="J17" s="137" t="s">
+      <c r="I17" s="129"/>
+      <c r="J17" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K17" s="130" t="s">
+      <c r="K17" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L17" s="130" t="s">
+      <c r="L17" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M17" s="151"/>
-      <c r="N17" s="147"/>
-      <c r="O17" s="132"/>
+      <c r="M17" s="152"/>
+      <c r="N17" s="148"/>
+      <c r="O17" s="133"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="134"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="136"/>
-      <c r="F18" s="138"/>
-      <c r="G18" s="126" t="n">
+      <c r="A18" s="135"/>
+      <c r="B18" s="136"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
+      <c r="E18" s="137"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="127" t="n">
         <v>33</v>
       </c>
-      <c r="H18" s="127" t="s">
+      <c r="H18" s="128" t="s">
         <v>257</v>
       </c>
-      <c r="I18" s="128"/>
-      <c r="J18" s="137" t="s">
+      <c r="I18" s="129"/>
+      <c r="J18" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K18" s="130" t="s">
+      <c r="K18" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L18" s="130" t="s">
+      <c r="L18" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M18" s="151"/>
-      <c r="N18" s="147"/>
-      <c r="O18" s="132"/>
+      <c r="M18" s="152"/>
+      <c r="N18" s="148"/>
+      <c r="O18" s="133"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="134"/>
-      <c r="B19" s="135"/>
-      <c r="C19" s="136"/>
-      <c r="D19" s="136"/>
-      <c r="E19" s="136"/>
-      <c r="F19" s="138"/>
-      <c r="G19" s="126" t="n">
+      <c r="A19" s="135"/>
+      <c r="B19" s="136"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
+      <c r="E19" s="137"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="127" t="n">
         <v>34</v>
       </c>
-      <c r="H19" s="127" t="s">
+      <c r="H19" s="128" t="s">
         <v>258</v>
       </c>
-      <c r="I19" s="128"/>
-      <c r="J19" s="137" t="s">
+      <c r="I19" s="129"/>
+      <c r="J19" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K19" s="130" t="s">
+      <c r="K19" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L19" s="130" t="s">
+      <c r="L19" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M19" s="151"/>
-      <c r="N19" s="147"/>
-      <c r="O19" s="132"/>
+      <c r="M19" s="152"/>
+      <c r="N19" s="148"/>
+      <c r="O19" s="133"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="134"/>
-      <c r="B20" s="135"/>
-      <c r="C20" s="136"/>
-      <c r="D20" s="136"/>
-      <c r="E20" s="136"/>
-      <c r="F20" s="138"/>
-      <c r="G20" s="126" t="n">
+      <c r="A20" s="135"/>
+      <c r="B20" s="136"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
+      <c r="E20" s="137"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="127" t="n">
         <v>35</v>
       </c>
-      <c r="H20" s="127" t="s">
+      <c r="H20" s="128" t="s">
         <v>259</v>
       </c>
-      <c r="I20" s="128"/>
-      <c r="J20" s="137" t="s">
+      <c r="I20" s="129"/>
+      <c r="J20" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K20" s="130" t="s">
+      <c r="K20" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L20" s="130" t="s">
+      <c r="L20" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M20" s="151"/>
-      <c r="N20" s="147"/>
-      <c r="O20" s="132"/>
+      <c r="M20" s="152"/>
+      <c r="N20" s="148"/>
+      <c r="O20" s="133"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="134"/>
-      <c r="B21" s="135"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="136"/>
-      <c r="F21" s="138"/>
-      <c r="G21" s="126" t="n">
+      <c r="A21" s="135"/>
+      <c r="B21" s="136"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
+      <c r="E21" s="137"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="127" t="n">
         <v>36</v>
       </c>
-      <c r="H21" s="127" t="s">
+      <c r="H21" s="128" t="s">
         <v>260</v>
       </c>
-      <c r="I21" s="128"/>
-      <c r="J21" s="137" t="s">
+      <c r="I21" s="129"/>
+      <c r="J21" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K21" s="130" t="s">
+      <c r="K21" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L21" s="130" t="s">
+      <c r="L21" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M21" s="151"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="132"/>
+      <c r="M21" s="152"/>
+      <c r="N21" s="148"/>
+      <c r="O21" s="133"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="134"/>
-      <c r="B22" s="135"/>
-      <c r="C22" s="136"/>
-      <c r="D22" s="136"/>
-      <c r="E22" s="136"/>
-      <c r="F22" s="138"/>
-      <c r="G22" s="126" t="n">
+      <c r="A22" s="135"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
+      <c r="E22" s="137"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="127" t="n">
         <v>37</v>
       </c>
-      <c r="H22" s="127" t="s">
+      <c r="H22" s="128" t="s">
         <v>261</v>
       </c>
-      <c r="I22" s="128"/>
-      <c r="J22" s="137" t="s">
+      <c r="I22" s="129"/>
+      <c r="J22" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K22" s="130" t="s">
+      <c r="K22" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L22" s="130" t="s">
+      <c r="L22" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M22" s="151"/>
-      <c r="N22" s="147"/>
-      <c r="O22" s="132"/>
+      <c r="M22" s="152"/>
+      <c r="N22" s="148"/>
+      <c r="O22" s="133"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="134"/>
-      <c r="B23" s="135"/>
-      <c r="C23" s="136"/>
-      <c r="D23" s="136"/>
-      <c r="E23" s="136"/>
-      <c r="F23" s="138"/>
-      <c r="G23" s="126" t="n">
+      <c r="A23" s="135"/>
+      <c r="B23" s="136"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
+      <c r="E23" s="137"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="127" t="n">
         <v>38</v>
       </c>
-      <c r="H23" s="127" t="s">
+      <c r="H23" s="128" t="s">
         <v>262</v>
       </c>
-      <c r="I23" s="128"/>
-      <c r="J23" s="137" t="s">
+      <c r="I23" s="129"/>
+      <c r="J23" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K23" s="130" t="s">
+      <c r="K23" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L23" s="130" t="s">
+      <c r="L23" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M23" s="151"/>
-      <c r="N23" s="147"/>
-      <c r="O23" s="132"/>
+      <c r="M23" s="152"/>
+      <c r="N23" s="148"/>
+      <c r="O23" s="133"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="134"/>
-      <c r="B24" s="135"/>
-      <c r="C24" s="136"/>
-      <c r="D24" s="136"/>
-      <c r="E24" s="136"/>
-      <c r="F24" s="138"/>
-      <c r="G24" s="126" t="n">
+      <c r="A24" s="135"/>
+      <c r="B24" s="136"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
+      <c r="E24" s="137"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="127" t="n">
         <v>39</v>
       </c>
-      <c r="H24" s="127" t="s">
+      <c r="H24" s="128" t="s">
         <v>263</v>
       </c>
-      <c r="I24" s="128"/>
-      <c r="J24" s="137" t="s">
+      <c r="I24" s="129"/>
+      <c r="J24" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K24" s="130" t="s">
+      <c r="K24" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L24" s="130" t="s">
+      <c r="L24" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M24" s="151"/>
-      <c r="N24" s="147"/>
-      <c r="O24" s="132"/>
+      <c r="M24" s="152"/>
+      <c r="N24" s="148"/>
+      <c r="O24" s="133"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="139"/>
-      <c r="B25" s="140"/>
-      <c r="C25" s="141"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="141"/>
-      <c r="F25" s="142"/>
-      <c r="G25" s="143" t="n">
+      <c r="A25" s="140"/>
+      <c r="B25" s="141"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="142"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="143"/>
+      <c r="G25" s="144" t="n">
         <v>4</v>
       </c>
-      <c r="H25" s="144" t="s">
+      <c r="H25" s="145" t="s">
         <v>264</v>
       </c>
-      <c r="I25" s="145"/>
-      <c r="J25" s="150"/>
-      <c r="K25" s="122"/>
-      <c r="L25" s="122"/>
-      <c r="M25" s="122"/>
-      <c r="N25" s="122"/>
-      <c r="O25" s="122"/>
+      <c r="I25" s="146"/>
+      <c r="J25" s="151"/>
+      <c r="K25" s="123"/>
+      <c r="L25" s="123"/>
+      <c r="M25" s="123"/>
+      <c r="N25" s="123"/>
+      <c r="O25" s="123"/>
     </row>
     <row r="26" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="134" t="s">
+      <c r="A26" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="135" t="s">
+      <c r="B26" s="136" t="s">
         <v>224</v>
       </c>
-      <c r="C26" s="136" t="s">
+      <c r="C26" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="D26" s="136" t="s">
+      <c r="D26" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="136"/>
-      <c r="F26" s="138" t="s">
+      <c r="E26" s="137"/>
+      <c r="F26" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G26" s="126" t="n">
+      <c r="G26" s="127" t="n">
         <v>41</v>
       </c>
-      <c r="H26" s="127" t="s">
+      <c r="H26" s="128" t="s">
         <v>265</v>
       </c>
-      <c r="I26" s="128"/>
-      <c r="J26" s="137" t="s">
+      <c r="I26" s="129"/>
+      <c r="J26" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K26" s="130" t="s">
+      <c r="K26" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L26" s="130" t="s">
+      <c r="L26" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M26" s="151" t="s">
+      <c r="M26" s="152" t="s">
         <v>266</v>
       </c>
-      <c r="N26" s="147" t="s">
+      <c r="N26" s="148" t="s">
         <v>267</v>
       </c>
-      <c r="O26" s="132"/>
+      <c r="O26" s="133"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="134"/>
-      <c r="B27" s="135"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="138"/>
-      <c r="G27" s="126" t="n">
+      <c r="A27" s="135"/>
+      <c r="B27" s="136"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="127" t="n">
         <v>42</v>
       </c>
-      <c r="H27" s="127" t="s">
+      <c r="H27" s="128" t="s">
         <v>268</v>
       </c>
-      <c r="I27" s="128"/>
-      <c r="J27" s="137" t="s">
+      <c r="I27" s="129"/>
+      <c r="J27" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K27" s="130" t="s">
+      <c r="K27" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L27" s="130" t="s">
+      <c r="L27" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M27" s="151"/>
-      <c r="N27" s="147"/>
-      <c r="O27" s="132"/>
+      <c r="M27" s="152"/>
+      <c r="N27" s="148"/>
+      <c r="O27" s="133"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="134"/>
-      <c r="B28" s="135"/>
-      <c r="C28" s="136"/>
-      <c r="D28" s="136"/>
-      <c r="E28" s="136"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="126" t="n">
+      <c r="A28" s="135"/>
+      <c r="B28" s="136"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
+      <c r="E28" s="137"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="127" t="n">
         <v>43</v>
       </c>
-      <c r="H28" s="127" t="s">
+      <c r="H28" s="128" t="s">
         <v>269</v>
       </c>
-      <c r="I28" s="128"/>
-      <c r="J28" s="137" t="s">
+      <c r="I28" s="129"/>
+      <c r="J28" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K28" s="130" t="s">
+      <c r="K28" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L28" s="130" t="s">
+      <c r="L28" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M28" s="151"/>
-      <c r="N28" s="147"/>
-      <c r="O28" s="132"/>
+      <c r="M28" s="152"/>
+      <c r="N28" s="148"/>
+      <c r="O28" s="133"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="134"/>
-      <c r="B29" s="135"/>
-      <c r="C29" s="136"/>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="138"/>
-      <c r="G29" s="126" t="n">
+      <c r="A29" s="135"/>
+      <c r="B29" s="136"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
+      <c r="E29" s="137"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="127" t="n">
         <v>44</v>
       </c>
-      <c r="H29" s="127" t="s">
+      <c r="H29" s="128" t="s">
         <v>270</v>
       </c>
-      <c r="I29" s="128"/>
-      <c r="J29" s="137" t="s">
+      <c r="I29" s="129"/>
+      <c r="J29" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K29" s="130" t="s">
+      <c r="K29" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L29" s="130" t="s">
+      <c r="L29" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M29" s="151"/>
-      <c r="N29" s="147"/>
-      <c r="O29" s="132"/>
+      <c r="M29" s="152"/>
+      <c r="N29" s="148"/>
+      <c r="O29" s="133"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="134"/>
-      <c r="B30" s="135"/>
-      <c r="C30" s="136"/>
-      <c r="D30" s="136"/>
-      <c r="E30" s="136"/>
-      <c r="F30" s="138"/>
-      <c r="G30" s="126" t="n">
+      <c r="A30" s="135"/>
+      <c r="B30" s="136"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="127" t="n">
         <v>45</v>
       </c>
-      <c r="H30" s="127" t="s">
+      <c r="H30" s="128" t="s">
         <v>271</v>
       </c>
-      <c r="I30" s="128"/>
-      <c r="J30" s="137" t="s">
+      <c r="I30" s="129"/>
+      <c r="J30" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K30" s="130" t="s">
+      <c r="K30" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L30" s="130" t="s">
+      <c r="L30" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M30" s="151"/>
-      <c r="N30" s="147"/>
-      <c r="O30" s="132"/>
+      <c r="M30" s="152"/>
+      <c r="N30" s="148"/>
+      <c r="O30" s="133"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="134"/>
-      <c r="B31" s="135"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="126" t="n">
+      <c r="A31" s="135"/>
+      <c r="B31" s="136"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="127" t="n">
         <v>46</v>
       </c>
-      <c r="H31" s="127" t="s">
+      <c r="H31" s="128" t="s">
         <v>272</v>
       </c>
-      <c r="I31" s="128"/>
-      <c r="J31" s="137" t="s">
+      <c r="I31" s="129"/>
+      <c r="J31" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K31" s="130" t="s">
+      <c r="K31" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L31" s="130" t="s">
+      <c r="L31" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M31" s="151"/>
-      <c r="N31" s="147"/>
-      <c r="O31" s="132"/>
+      <c r="M31" s="152"/>
+      <c r="N31" s="148"/>
+      <c r="O31" s="133"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="134"/>
-      <c r="B32" s="135"/>
-      <c r="C32" s="136"/>
-      <c r="D32" s="136"/>
-      <c r="E32" s="136"/>
-      <c r="F32" s="138"/>
-      <c r="G32" s="126" t="n">
+      <c r="A32" s="135"/>
+      <c r="B32" s="136"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
+      <c r="E32" s="137"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="127" t="n">
         <v>47</v>
       </c>
-      <c r="H32" s="127" t="s">
+      <c r="H32" s="128" t="s">
         <v>273</v>
       </c>
-      <c r="I32" s="128"/>
-      <c r="J32" s="137" t="s">
+      <c r="I32" s="129"/>
+      <c r="J32" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K32" s="130" t="s">
+      <c r="K32" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L32" s="130" t="s">
+      <c r="L32" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M32" s="151"/>
-      <c r="N32" s="147"/>
-      <c r="O32" s="132"/>
+      <c r="M32" s="152"/>
+      <c r="N32" s="148"/>
+      <c r="O32" s="133"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="134"/>
-      <c r="B33" s="135"/>
-      <c r="C33" s="136"/>
-      <c r="D33" s="136"/>
-      <c r="E33" s="136"/>
-      <c r="F33" s="138"/>
-      <c r="G33" s="126" t="n">
+      <c r="A33" s="135"/>
+      <c r="B33" s="136"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="137"/>
+      <c r="F33" s="139"/>
+      <c r="G33" s="127" t="n">
         <v>48</v>
       </c>
-      <c r="H33" s="127" t="s">
+      <c r="H33" s="128" t="s">
         <v>274</v>
       </c>
-      <c r="I33" s="128"/>
-      <c r="J33" s="137" t="s">
+      <c r="I33" s="129"/>
+      <c r="J33" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K33" s="130" t="s">
+      <c r="K33" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L33" s="130" t="s">
+      <c r="L33" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M33" s="151"/>
-      <c r="N33" s="147"/>
-      <c r="O33" s="132"/>
+      <c r="M33" s="152"/>
+      <c r="N33" s="148"/>
+      <c r="O33" s="133"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="134"/>
-      <c r="B34" s="135"/>
-      <c r="C34" s="136"/>
-      <c r="D34" s="136"/>
-      <c r="E34" s="136"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="126" t="n">
+      <c r="A34" s="135"/>
+      <c r="B34" s="136"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
+      <c r="E34" s="137"/>
+      <c r="F34" s="139"/>
+      <c r="G34" s="127" t="n">
         <v>49</v>
       </c>
-      <c r="H34" s="127" t="s">
+      <c r="H34" s="128" t="s">
         <v>275</v>
       </c>
-      <c r="I34" s="128"/>
-      <c r="J34" s="137" t="s">
+      <c r="I34" s="129"/>
+      <c r="J34" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K34" s="130" t="s">
+      <c r="K34" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L34" s="130" t="s">
+      <c r="L34" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M34" s="151"/>
-      <c r="N34" s="147"/>
-      <c r="O34" s="132"/>
+      <c r="M34" s="152"/>
+      <c r="N34" s="148"/>
+      <c r="O34" s="133"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="139"/>
-      <c r="B35" s="140"/>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="142"/>
-      <c r="G35" s="143" t="n">
+      <c r="A35" s="140"/>
+      <c r="B35" s="141"/>
+      <c r="C35" s="142"/>
+      <c r="D35" s="142"/>
+      <c r="E35" s="142"/>
+      <c r="F35" s="143"/>
+      <c r="G35" s="144" t="n">
         <v>5</v>
       </c>
-      <c r="H35" s="144" t="s">
+      <c r="H35" s="145" t="s">
         <v>276</v>
       </c>
-      <c r="I35" s="145"/>
-      <c r="J35" s="150"/>
-      <c r="K35" s="122"/>
-      <c r="L35" s="122"/>
-      <c r="M35" s="122"/>
-      <c r="N35" s="122"/>
-      <c r="O35" s="122"/>
+      <c r="I35" s="146"/>
+      <c r="J35" s="151"/>
+      <c r="K35" s="123"/>
+      <c r="L35" s="123"/>
+      <c r="M35" s="123"/>
+      <c r="N35" s="123"/>
+      <c r="O35" s="123"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="134"/>
-      <c r="B36" s="135"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="136"/>
-      <c r="F36" s="138"/>
-      <c r="G36" s="126" t="n">
+      <c r="A36" s="135"/>
+      <c r="B36" s="136"/>
+      <c r="C36" s="137"/>
+      <c r="D36" s="137"/>
+      <c r="E36" s="137"/>
+      <c r="F36" s="139"/>
+      <c r="G36" s="127" t="n">
         <v>51</v>
       </c>
-      <c r="H36" s="127" t="s">
+      <c r="H36" s="128" t="s">
         <v>277</v>
       </c>
-      <c r="I36" s="137" t="s">
+      <c r="I36" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J36" s="128"/>
-      <c r="K36" s="132"/>
-      <c r="L36" s="132"/>
-      <c r="M36" s="152"/>
-      <c r="N36" s="152"/>
-      <c r="O36" s="152"/>
+      <c r="J36" s="129"/>
+      <c r="K36" s="133"/>
+      <c r="L36" s="133"/>
+      <c r="M36" s="153"/>
+      <c r="N36" s="153"/>
+      <c r="O36" s="153"/>
     </row>
     <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="134"/>
-      <c r="B37" s="135"/>
-      <c r="C37" s="136"/>
-      <c r="D37" s="136" t="s">
+      <c r="A37" s="135"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="137"/>
+      <c r="D37" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E37" s="136"/>
-      <c r="F37" s="138"/>
-      <c r="G37" s="126" t="n">
+      <c r="E37" s="137"/>
+      <c r="F37" s="139"/>
+      <c r="G37" s="127" t="n">
         <v>52</v>
       </c>
-      <c r="H37" s="127" t="s">
+      <c r="H37" s="128" t="s">
         <v>278</v>
       </c>
-      <c r="I37" s="128"/>
-      <c r="J37" s="129" t="s">
+      <c r="I37" s="129"/>
+      <c r="J37" s="130" t="s">
         <v>279</v>
       </c>
-      <c r="K37" s="130" t="s">
+      <c r="K37" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L37" s="130" t="s">
+      <c r="L37" s="131" t="s">
         <v>242</v>
       </c>
-      <c r="M37" s="131" t="s">
+      <c r="M37" s="132" t="s">
         <v>280</v>
       </c>
-      <c r="N37" s="131" t="s">
+      <c r="N37" s="132" t="s">
         <v>281</v>
       </c>
-      <c r="O37" s="152"/>
+      <c r="O37" s="153"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="134"/>
-      <c r="B38" s="135"/>
-      <c r="C38" s="136"/>
-      <c r="D38" s="136"/>
-      <c r="E38" s="136"/>
-      <c r="F38" s="138"/>
-      <c r="G38" s="126" t="n">
+      <c r="A38" s="135"/>
+      <c r="B38" s="136"/>
+      <c r="C38" s="137"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="137"/>
+      <c r="F38" s="139"/>
+      <c r="G38" s="127" t="n">
         <v>53</v>
       </c>
-      <c r="H38" s="127" t="s">
+      <c r="H38" s="128" t="s">
         <v>282</v>
       </c>
-      <c r="I38" s="137" t="s">
+      <c r="I38" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J38" s="128"/>
-      <c r="K38" s="132"/>
-      <c r="L38" s="132"/>
-      <c r="M38" s="152"/>
-      <c r="N38" s="152"/>
-      <c r="O38" s="152"/>
+      <c r="J38" s="129"/>
+      <c r="K38" s="133"/>
+      <c r="L38" s="133"/>
+      <c r="M38" s="153"/>
+      <c r="N38" s="153"/>
+      <c r="O38" s="153"/>
     </row>
     <row r="39" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="B39" s="135"/>
-      <c r="C39" s="136"/>
-      <c r="D39" s="136" t="s">
+      <c r="B39" s="136"/>
+      <c r="C39" s="137"/>
+      <c r="D39" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E39" s="136"/>
-      <c r="F39" s="138"/>
-      <c r="G39" s="126" t="n">
+      <c r="E39" s="137"/>
+      <c r="F39" s="139"/>
+      <c r="G39" s="127" t="n">
         <v>54</v>
       </c>
-      <c r="H39" s="127" t="s">
+      <c r="H39" s="128" t="s">
         <v>283</v>
       </c>
-      <c r="I39" s="128"/>
-      <c r="J39" s="129" t="s">
+      <c r="I39" s="129"/>
+      <c r="J39" s="130" t="s">
         <v>284</v>
       </c>
-      <c r="K39" s="130" t="s">
+      <c r="K39" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L39" s="130" t="s">
+      <c r="L39" s="131" t="s">
         <v>285</v>
       </c>
-      <c r="M39" s="131" t="s">
+      <c r="M39" s="132" t="s">
         <v>286</v>
       </c>
-      <c r="N39" s="131" t="s">
+      <c r="N39" s="132" t="s">
         <v>287</v>
       </c>
-      <c r="O39" s="152"/>
+      <c r="O39" s="153"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="134"/>
-      <c r="B40" s="135"/>
-      <c r="C40" s="136"/>
-      <c r="D40" s="136"/>
-      <c r="E40" s="136"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="126" t="n">
+      <c r="A40" s="135"/>
+      <c r="B40" s="136"/>
+      <c r="C40" s="137"/>
+      <c r="D40" s="137"/>
+      <c r="E40" s="137"/>
+      <c r="F40" s="139"/>
+      <c r="G40" s="127" t="n">
         <v>55</v>
       </c>
-      <c r="H40" s="127" t="s">
+      <c r="H40" s="128" t="s">
         <v>288</v>
       </c>
-      <c r="I40" s="128"/>
-      <c r="J40" s="129" t="s">
+      <c r="I40" s="129"/>
+      <c r="J40" s="130" t="s">
         <v>279</v>
       </c>
-      <c r="K40" s="130" t="s">
+      <c r="K40" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L40" s="130" t="s">
+      <c r="L40" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M40" s="152"/>
-      <c r="N40" s="152"/>
-      <c r="O40" s="152"/>
+      <c r="M40" s="153"/>
+      <c r="N40" s="153"/>
+      <c r="O40" s="153"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="134"/>
-      <c r="B41" s="135"/>
-      <c r="C41" s="136"/>
-      <c r="D41" s="136"/>
-      <c r="E41" s="136"/>
-      <c r="F41" s="138"/>
-      <c r="G41" s="126" t="n">
+      <c r="A41" s="135"/>
+      <c r="B41" s="136"/>
+      <c r="C41" s="137"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="137"/>
+      <c r="F41" s="139"/>
+      <c r="G41" s="127" t="n">
         <v>56</v>
       </c>
-      <c r="H41" s="127" t="s">
+      <c r="H41" s="128" t="s">
         <v>289</v>
       </c>
-      <c r="I41" s="128"/>
-      <c r="J41" s="129" t="s">
+      <c r="I41" s="129"/>
+      <c r="J41" s="130" t="s">
         <v>279</v>
       </c>
-      <c r="K41" s="130" t="s">
+      <c r="K41" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="130" t="s">
+      <c r="L41" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M41" s="152"/>
-      <c r="N41" s="152"/>
-      <c r="O41" s="152"/>
+      <c r="M41" s="153"/>
+      <c r="N41" s="153"/>
+      <c r="O41" s="153"/>
     </row>
     <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="134"/>
-      <c r="B42" s="135"/>
-      <c r="C42" s="136"/>
-      <c r="D42" s="136"/>
-      <c r="E42" s="136"/>
-      <c r="F42" s="138"/>
-      <c r="G42" s="126" t="n">
+      <c r="A42" s="135"/>
+      <c r="B42" s="136"/>
+      <c r="C42" s="137"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="139"/>
+      <c r="G42" s="127" t="n">
         <v>57</v>
       </c>
-      <c r="H42" s="127" t="s">
+      <c r="H42" s="128" t="s">
         <v>290</v>
       </c>
-      <c r="I42" s="128"/>
-      <c r="J42" s="129" t="s">
+      <c r="I42" s="129"/>
+      <c r="J42" s="130" t="s">
         <v>291</v>
       </c>
-      <c r="K42" s="130" t="s">
+      <c r="K42" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L42" s="130" t="s">
+      <c r="L42" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M42" s="152"/>
-      <c r="N42" s="152"/>
-      <c r="O42" s="152"/>
+      <c r="M42" s="153"/>
+      <c r="N42" s="153"/>
+      <c r="O42" s="153"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="139"/>
-      <c r="B43" s="140"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="141"/>
-      <c r="E43" s="141"/>
-      <c r="F43" s="142"/>
-      <c r="G43" s="143" t="n">
+      <c r="A43" s="140"/>
+      <c r="B43" s="141"/>
+      <c r="C43" s="142"/>
+      <c r="D43" s="142"/>
+      <c r="E43" s="142"/>
+      <c r="F43" s="143"/>
+      <c r="G43" s="144" t="n">
         <v>6</v>
       </c>
-      <c r="H43" s="144" t="s">
+      <c r="H43" s="145" t="s">
         <v>292</v>
       </c>
-      <c r="I43" s="145"/>
-      <c r="J43" s="150"/>
-      <c r="K43" s="122"/>
-      <c r="L43" s="122"/>
-      <c r="M43" s="122"/>
-      <c r="N43" s="122"/>
-      <c r="O43" s="122"/>
+      <c r="I43" s="146"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="123"/>
+      <c r="L43" s="123"/>
+      <c r="M43" s="123"/>
+      <c r="N43" s="123"/>
+      <c r="O43" s="123"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="134"/>
-      <c r="B44" s="135"/>
-      <c r="C44" s="136"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="136"/>
-      <c r="F44" s="138"/>
-      <c r="G44" s="126" t="n">
+      <c r="A44" s="135"/>
+      <c r="B44" s="136"/>
+      <c r="C44" s="137"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="137"/>
+      <c r="F44" s="139"/>
+      <c r="G44" s="127" t="n">
         <v>61</v>
       </c>
-      <c r="H44" s="127" t="s">
+      <c r="H44" s="128" t="s">
         <v>293</v>
       </c>
-      <c r="I44" s="137" t="s">
+      <c r="I44" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J44" s="128"/>
-      <c r="K44" s="132"/>
-      <c r="L44" s="132"/>
-      <c r="M44" s="132"/>
-      <c r="N44" s="132"/>
-      <c r="O44" s="132"/>
+      <c r="J44" s="129"/>
+      <c r="K44" s="133"/>
+      <c r="L44" s="133"/>
+      <c r="M44" s="133"/>
+      <c r="N44" s="133"/>
+      <c r="O44" s="133"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="134" t="s">
+      <c r="A45" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="B45" s="135"/>
-      <c r="C45" s="136"/>
-      <c r="D45" s="136" t="s">
+      <c r="B45" s="136"/>
+      <c r="C45" s="137"/>
+      <c r="D45" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E45" s="136"/>
-      <c r="F45" s="138" t="s">
+      <c r="E45" s="137"/>
+      <c r="F45" s="139" t="s">
         <v>224</v>
       </c>
-      <c r="G45" s="126" t="n">
+      <c r="G45" s="127" t="n">
         <v>62</v>
       </c>
-      <c r="H45" s="127" t="s">
+      <c r="H45" s="128" t="s">
         <v>294</v>
       </c>
-      <c r="I45" s="128"/>
-      <c r="J45" s="129" t="s">
+      <c r="I45" s="129"/>
+      <c r="J45" s="130" t="s">
         <v>279</v>
       </c>
-      <c r="K45" s="130" t="s">
+      <c r="K45" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L45" s="130" t="s">
+      <c r="L45" s="131" t="s">
         <v>228</v>
       </c>
-      <c r="M45" s="130" t="s">
+      <c r="M45" s="131" t="s">
         <v>295</v>
       </c>
-      <c r="N45" s="132"/>
-      <c r="O45" s="132"/>
-      <c r="P45" s="153"/>
+      <c r="N45" s="133"/>
+      <c r="O45" s="133"/>
+      <c r="P45" s="154"/>
     </row>
     <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="134"/>
-      <c r="B46" s="135"/>
-      <c r="C46" s="136"/>
-      <c r="D46" s="136"/>
-      <c r="E46" s="136"/>
-      <c r="F46" s="138"/>
-      <c r="G46" s="126" t="n">
+      <c r="A46" s="135"/>
+      <c r="B46" s="136"/>
+      <c r="C46" s="137"/>
+      <c r="D46" s="137"/>
+      <c r="E46" s="137"/>
+      <c r="F46" s="139"/>
+      <c r="G46" s="127" t="n">
         <v>63</v>
       </c>
-      <c r="H46" s="127" t="s">
+      <c r="H46" s="128" t="s">
         <v>296</v>
       </c>
-      <c r="I46" s="128"/>
-      <c r="J46" s="129" t="s">
+      <c r="I46" s="129"/>
+      <c r="J46" s="130" t="s">
         <v>297</v>
       </c>
-      <c r="K46" s="130" t="s">
+      <c r="K46" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L46" s="130" t="s">
+      <c r="L46" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M46" s="132"/>
-      <c r="N46" s="132"/>
-      <c r="O46" s="132"/>
+      <c r="M46" s="133"/>
+      <c r="N46" s="133"/>
+      <c r="O46" s="133"/>
     </row>
     <row r="47" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="139"/>
-      <c r="B47" s="140"/>
-      <c r="C47" s="141"/>
-      <c r="D47" s="141"/>
-      <c r="E47" s="141"/>
-      <c r="F47" s="142"/>
-      <c r="G47" s="143" t="n">
+      <c r="A47" s="140"/>
+      <c r="B47" s="141"/>
+      <c r="C47" s="142"/>
+      <c r="D47" s="142"/>
+      <c r="E47" s="142"/>
+      <c r="F47" s="143"/>
+      <c r="G47" s="144" t="n">
         <v>7</v>
       </c>
-      <c r="H47" s="144" t="s">
+      <c r="H47" s="145" t="s">
         <v>298</v>
       </c>
-      <c r="I47" s="145"/>
-      <c r="J47" s="150"/>
-      <c r="K47" s="122"/>
-      <c r="L47" s="122"/>
-      <c r="M47" s="154" t="s">
+      <c r="I47" s="146"/>
+      <c r="J47" s="151"/>
+      <c r="K47" s="123"/>
+      <c r="L47" s="123"/>
+      <c r="M47" s="155" t="s">
         <v>299</v>
       </c>
-      <c r="N47" s="154" t="s">
+      <c r="N47" s="155" t="s">
         <v>300</v>
       </c>
-      <c r="O47" s="154" t="s">
+      <c r="O47" s="155" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="134"/>
-      <c r="B48" s="135"/>
-      <c r="C48" s="136"/>
-      <c r="D48" s="136" t="s">
+      <c r="A48" s="135"/>
+      <c r="B48" s="136"/>
+      <c r="C48" s="137"/>
+      <c r="D48" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E48" s="136" t="s">
+      <c r="E48" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="F48" s="136"/>
-      <c r="G48" s="126" t="n">
+      <c r="F48" s="137"/>
+      <c r="G48" s="127" t="n">
         <v>71</v>
       </c>
-      <c r="H48" s="127" t="s">
+      <c r="H48" s="128" t="s">
         <v>302</v>
       </c>
-      <c r="I48" s="128"/>
-      <c r="J48" s="129" t="s">
+      <c r="I48" s="129"/>
+      <c r="J48" s="130" t="s">
         <v>303</v>
       </c>
-      <c r="K48" s="130" t="s">
+      <c r="K48" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L48" s="130" t="s">
+      <c r="L48" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="M48" s="130" t="s">
+      <c r="M48" s="131" t="s">
         <v>305</v>
       </c>
-      <c r="N48" s="130" t="s">
+      <c r="N48" s="131" t="s">
         <v>305</v>
       </c>
-      <c r="O48" s="130" t="s">
+      <c r="O48" s="131" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="134"/>
-      <c r="B49" s="135"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136" t="s">
+      <c r="A49" s="135"/>
+      <c r="B49" s="136"/>
+      <c r="C49" s="137"/>
+      <c r="D49" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E49" s="136" t="s">
+      <c r="E49" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="F49" s="136" t="s">
+      <c r="F49" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="G49" s="126" t="n">
+      <c r="G49" s="127" t="n">
         <v>72</v>
       </c>
-      <c r="H49" s="127" t="s">
+      <c r="H49" s="128" t="s">
         <v>306</v>
       </c>
-      <c r="I49" s="128"/>
-      <c r="J49" s="129" t="s">
+      <c r="I49" s="129"/>
+      <c r="J49" s="130" t="s">
         <v>307</v>
       </c>
-      <c r="K49" s="130" t="s">
+      <c r="K49" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L49" s="130" t="s">
+      <c r="L49" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="M49" s="130" t="s">
+      <c r="M49" s="131" t="s">
         <v>308</v>
       </c>
-      <c r="N49" s="130" t="s">
+      <c r="N49" s="131" t="s">
         <v>308</v>
       </c>
-      <c r="O49" s="130" t="s">
+      <c r="O49" s="131" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="134"/>
-      <c r="B50" s="135"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136" t="s">
+      <c r="A50" s="135"/>
+      <c r="B50" s="136"/>
+      <c r="C50" s="137"/>
+      <c r="D50" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="E50" s="136" t="s">
+      <c r="E50" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="F50" s="136" t="s">
+      <c r="F50" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="G50" s="126" t="n">
+      <c r="G50" s="127" t="n">
         <v>73</v>
       </c>
-      <c r="H50" s="127" t="s">
+      <c r="H50" s="128" t="s">
         <v>309</v>
       </c>
-      <c r="I50" s="128"/>
-      <c r="J50" s="129" t="s">
+      <c r="I50" s="129"/>
+      <c r="J50" s="130" t="s">
         <v>310</v>
       </c>
-      <c r="K50" s="130" t="s">
+      <c r="K50" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L50" s="130" t="s">
+      <c r="L50" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="M50" s="130" t="s">
+      <c r="M50" s="131" t="s">
         <v>311</v>
       </c>
-      <c r="N50" s="130" t="s">
+      <c r="N50" s="131" t="s">
         <v>311</v>
       </c>
-      <c r="O50" s="130" t="s">
+      <c r="O50" s="131" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="134"/>
-      <c r="B51" s="135"/>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="136"/>
-      <c r="F51" s="136" t="s">
+      <c r="A51" s="135"/>
+      <c r="B51" s="136"/>
+      <c r="C51" s="137"/>
+      <c r="D51" s="137"/>
+      <c r="E51" s="137"/>
+      <c r="F51" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="G51" s="126" t="n">
+      <c r="G51" s="127" t="n">
         <v>74</v>
       </c>
-      <c r="H51" s="127" t="s">
+      <c r="H51" s="128" t="s">
         <v>312</v>
       </c>
-      <c r="I51" s="128"/>
-      <c r="J51" s="129" t="s">
+      <c r="I51" s="129"/>
+      <c r="J51" s="130" t="s">
         <v>313</v>
       </c>
-      <c r="K51" s="130" t="s">
+      <c r="K51" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L51" s="130" t="s">
+      <c r="L51" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="M51" s="130" t="s">
+      <c r="M51" s="131" t="s">
         <v>314</v>
       </c>
-      <c r="N51" s="130" t="s">
+      <c r="N51" s="131" t="s">
         <v>314</v>
       </c>
-      <c r="O51" s="130" t="s">
+      <c r="O51" s="131" t="s">
         <v>314</v>
       </c>
-      <c r="P51" s="153"/>
+      <c r="P51" s="154"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="134"/>
-      <c r="B52" s="135"/>
-      <c r="C52" s="136"/>
-      <c r="D52" s="136"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="136" t="s">
+      <c r="A52" s="135"/>
+      <c r="B52" s="136"/>
+      <c r="C52" s="137"/>
+      <c r="D52" s="137"/>
+      <c r="E52" s="137"/>
+      <c r="F52" s="137" t="s">
         <v>224</v>
       </c>
-      <c r="G52" s="126" t="n">
+      <c r="G52" s="127" t="n">
         <v>75</v>
       </c>
-      <c r="H52" s="127" t="s">
+      <c r="H52" s="128" t="s">
         <v>315</v>
       </c>
-      <c r="I52" s="128"/>
-      <c r="J52" s="129" t="s">
+      <c r="I52" s="129"/>
+      <c r="J52" s="130" t="s">
         <v>316</v>
       </c>
-      <c r="K52" s="130" t="s">
+      <c r="K52" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L52" s="130" t="s">
+      <c r="L52" s="131" t="s">
         <v>304</v>
       </c>
-      <c r="M52" s="130" t="s">
+      <c r="M52" s="131" t="s">
         <v>317</v>
       </c>
-      <c r="N52" s="130" t="s">
+      <c r="N52" s="131" t="s">
         <v>317</v>
       </c>
-      <c r="O52" s="130" t="s">
+      <c r="O52" s="131" t="s">
         <v>317</v>
       </c>
-      <c r="P52" s="153"/>
+      <c r="P52" s="154"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="139"/>
-      <c r="B53" s="140"/>
-      <c r="C53" s="141"/>
-      <c r="D53" s="141"/>
-      <c r="E53" s="141"/>
-      <c r="F53" s="142"/>
-      <c r="G53" s="143" t="n">
+      <c r="A53" s="140"/>
+      <c r="B53" s="141"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="142"/>
+      <c r="F53" s="143"/>
+      <c r="G53" s="144" t="n">
         <v>8</v>
       </c>
-      <c r="H53" s="144" t="s">
+      <c r="H53" s="145" t="s">
         <v>318</v>
       </c>
-      <c r="I53" s="145"/>
-      <c r="J53" s="150"/>
-      <c r="K53" s="122"/>
-      <c r="L53" s="122"/>
-      <c r="M53" s="122"/>
-      <c r="N53" s="122"/>
-      <c r="O53" s="122"/>
+      <c r="I53" s="146"/>
+      <c r="J53" s="151"/>
+      <c r="K53" s="123"/>
+      <c r="L53" s="123"/>
+      <c r="M53" s="123"/>
+      <c r="N53" s="123"/>
+      <c r="O53" s="123"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="134"/>
-      <c r="B54" s="135"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="136"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="138"/>
-      <c r="G54" s="126" t="n">
+      <c r="A54" s="135"/>
+      <c r="B54" s="136"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="137"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="139"/>
+      <c r="G54" s="127" t="n">
         <v>81</v>
       </c>
-      <c r="H54" s="127" t="s">
+      <c r="H54" s="128" t="s">
         <v>319</v>
       </c>
-      <c r="I54" s="137" t="s">
+      <c r="I54" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="J54" s="128"/>
-      <c r="K54" s="132"/>
-      <c r="L54" s="132"/>
-      <c r="M54" s="132"/>
-      <c r="N54" s="132"/>
-      <c r="O54" s="132"/>
+      <c r="J54" s="129"/>
+      <c r="K54" s="133"/>
+      <c r="L54" s="133"/>
+      <c r="M54" s="133"/>
+      <c r="N54" s="133"/>
+      <c r="O54" s="133"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="134"/>
-      <c r="B55" s="135"/>
-      <c r="C55" s="136"/>
-      <c r="D55" s="136"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="138"/>
-      <c r="G55" s="126" t="n">
+      <c r="A55" s="135"/>
+      <c r="B55" s="136"/>
+      <c r="C55" s="137"/>
+      <c r="D55" s="137"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="139"/>
+      <c r="G55" s="127" t="n">
         <v>82</v>
       </c>
-      <c r="H55" s="127" t="s">
+      <c r="H55" s="128" t="s">
         <v>320</v>
       </c>
-      <c r="I55" s="128"/>
-      <c r="J55" s="129" t="s">
+      <c r="I55" s="129"/>
+      <c r="J55" s="130" t="s">
         <v>321</v>
       </c>
-      <c r="K55" s="130" t="s">
+      <c r="K55" s="131" t="s">
         <v>23</v>
       </c>
-      <c r="L55" s="130" t="s">
+      <c r="L55" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M55" s="132"/>
-      <c r="N55" s="132"/>
-      <c r="O55" s="132"/>
+      <c r="M55" s="133"/>
+      <c r="N55" s="133"/>
+      <c r="O55" s="133"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="139"/>
-      <c r="B56" s="140"/>
-      <c r="C56" s="141"/>
-      <c r="D56" s="141"/>
-      <c r="E56" s="141"/>
-      <c r="F56" s="142"/>
-      <c r="G56" s="143" t="n">
+      <c r="A56" s="140"/>
+      <c r="B56" s="141"/>
+      <c r="C56" s="142"/>
+      <c r="D56" s="142"/>
+      <c r="E56" s="142"/>
+      <c r="F56" s="143"/>
+      <c r="G56" s="144" t="n">
         <v>9</v>
       </c>
-      <c r="H56" s="144" t="s">
+      <c r="H56" s="145" t="s">
         <v>322</v>
       </c>
-      <c r="I56" s="145"/>
-      <c r="J56" s="150"/>
-      <c r="K56" s="122"/>
-      <c r="L56" s="122"/>
-      <c r="M56" s="122"/>
-      <c r="N56" s="122"/>
-      <c r="O56" s="122"/>
+      <c r="I56" s="146"/>
+      <c r="J56" s="151"/>
+      <c r="K56" s="123"/>
+      <c r="L56" s="123"/>
+      <c r="M56" s="123"/>
+      <c r="N56" s="123"/>
+      <c r="O56" s="123"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="134"/>
-      <c r="B57" s="135"/>
-      <c r="C57" s="136"/>
-      <c r="D57" s="136"/>
-      <c r="E57" s="136"/>
-      <c r="F57" s="138"/>
-      <c r="G57" s="126" t="n">
+      <c r="A57" s="135"/>
+      <c r="B57" s="136"/>
+      <c r="C57" s="137"/>
+      <c r="D57" s="137"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="139"/>
+      <c r="G57" s="127" t="n">
         <v>91</v>
       </c>
-      <c r="H57" s="127" t="s">
+      <c r="H57" s="128" t="s">
         <v>323</v>
       </c>
-      <c r="I57" s="128"/>
-      <c r="J57" s="137" t="s">
+      <c r="I57" s="129"/>
+      <c r="J57" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K57" s="130" t="s">
+      <c r="K57" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L57" s="130" t="s">
+      <c r="L57" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M57" s="132"/>
-      <c r="N57" s="132"/>
-      <c r="O57" s="132"/>
+      <c r="M57" s="133"/>
+      <c r="N57" s="133"/>
+      <c r="O57" s="133"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="155"/>
-      <c r="B58" s="156"/>
-      <c r="C58" s="157"/>
-      <c r="D58" s="157"/>
-      <c r="E58" s="157"/>
-      <c r="F58" s="158"/>
-      <c r="G58" s="126" t="n">
+      <c r="A58" s="156"/>
+      <c r="B58" s="157"/>
+      <c r="C58" s="158"/>
+      <c r="D58" s="158"/>
+      <c r="E58" s="158"/>
+      <c r="F58" s="159"/>
+      <c r="G58" s="127" t="n">
         <v>92</v>
       </c>
-      <c r="H58" s="127" t="s">
+      <c r="H58" s="128" t="s">
         <v>324</v>
       </c>
-      <c r="I58" s="128"/>
-      <c r="J58" s="137" t="s">
+      <c r="I58" s="129"/>
+      <c r="J58" s="138" t="s">
         <v>232</v>
       </c>
-      <c r="K58" s="130" t="s">
+      <c r="K58" s="131" t="s">
         <v>227</v>
       </c>
-      <c r="L58" s="130" t="s">
+      <c r="L58" s="131" t="s">
         <v>236</v>
       </c>
-      <c r="M58" s="132"/>
-      <c r="N58" s="132"/>
-      <c r="O58" s="132"/>
+      <c r="M58" s="133"/>
+      <c r="N58" s="133"/>
+      <c r="O58" s="133"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="159"/>
-      <c r="B59" s="160"/>
-      <c r="C59" s="161"/>
-      <c r="D59" s="161"/>
-      <c r="E59" s="161"/>
-      <c r="F59" s="162"/>
-      <c r="G59" s="163" t="n">
+      <c r="A59" s="160"/>
+      <c r="B59" s="161"/>
+      <c r="C59" s="162"/>
+      <c r="D59" s="162"/>
+      <c r="E59" s="162"/>
+      <c r="F59" s="163"/>
+      <c r="G59" s="164" t="n">
         <v>93</v>
       </c>
-      <c r="H59" s="80" t="s">
+      <c r="H59" s="81" t="s">
         <v>325</v>
       </c>
-      <c r="I59" s="164" t="s">
+      <c r="I59" s="165" t="s">
         <v>326</v>
       </c>
-      <c r="J59" s="164" t="s">
+      <c r="J59" s="165" t="s">
         <v>326</v>
       </c>
-      <c r="K59" s="165" t="s">
+      <c r="K59" s="166" t="s">
         <v>326</v>
       </c>
-      <c r="L59" s="165" t="s">
+      <c r="L59" s="166" t="s">
         <v>304</v>
       </c>
-      <c r="M59" s="166" t="s">
+      <c r="M59" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="N59" s="166" t="s">
+      <c r="N59" s="167" t="s">
         <v>327</v>
       </c>
-      <c r="O59" s="166" t="s">
+      <c r="O59" s="167" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="60" s="167" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G60" s="153"/>
-      <c r="M60" s="168" t="s">
+    <row r="60" s="168" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G60" s="154"/>
+      <c r="M60" s="169" t="s">
         <v>328</v>
       </c>
-      <c r="N60" s="168"/>
-      <c r="O60" s="168"/>
-      <c r="P60" s="153"/>
-    </row>
-    <row r="61" s="167" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G61" s="153"/>
-      <c r="M61" s="169" t="s">
+      <c r="N60" s="169"/>
+      <c r="O60" s="169"/>
+      <c r="P60" s="154"/>
+    </row>
+    <row r="61" s="168" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G61" s="154"/>
+      <c r="M61" s="170" t="s">
         <v>329</v>
       </c>
-      <c r="N61" s="169"/>
-      <c r="O61" s="169"/>
-      <c r="P61" s="153"/>
+      <c r="N61" s="170"/>
+      <c r="O61" s="170"/>
+      <c r="P61" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>